<commit_message>
merge ws-infoHotel to Dev
</commit_message>
<xml_diff>
--- a/Database/hotel_management.xlsx
+++ b/Database/hotel_management.xlsx
@@ -383,10 +383,6 @@
 1 - Vip</t>
   </si>
   <si>
-    <t>0 - Non empty
-1 - Empty</t>
-  </si>
-  <si>
     <t>FK(Table)</t>
   </si>
   <si>
@@ -424,6 +420,10 @@
   </si>
   <si>
     <t>Yêu cầu của khách hàng</t>
+  </si>
+  <si>
+    <t>0 - Empty
+1 - Not Empty</t>
   </si>
 </sst>
 </file>
@@ -1228,8 +1228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C61" workbookViewId="0">
-      <selection activeCell="K67" sqref="K67"/>
+    <sheetView tabSelected="1" topLeftCell="B14" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1276,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>6</v>
@@ -1800,7 +1800,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="15" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.25">
@@ -1938,7 +1938,7 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="2:13" x14ac:dyDescent="0.25">
@@ -2122,7 +2122,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
       <c r="M49" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="2:13" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
       <c r="M54" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.25">
@@ -2640,7 +2640,7 @@
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
       <c r="M68" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="69" spans="2:13" x14ac:dyDescent="0.25">
@@ -2734,7 +2734,7 @@
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
       <c r="M73" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="74" spans="2:13" x14ac:dyDescent="0.25">
@@ -2916,7 +2916,7 @@
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
       <c r="M82" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="2:13" x14ac:dyDescent="0.25">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="L87" s="1"/>
       <c r="M87" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="88" spans="2:13" x14ac:dyDescent="0.25">
@@ -3220,7 +3220,7 @@
       </c>
       <c r="L97" s="13"/>
       <c r="M97" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>